<commit_message>
Change paths to excel files
</commit_message>
<xml_diff>
--- a/conversion.xlsx
+++ b/conversion.xlsx
@@ -366,19 +366,24 @@
           <t>odno</t>
         </is>
       </c>
-      <c r="E5" s="0" t="n">
-        <v>11111</v>
-      </c>
-      <c r="F5" s="0" t="n">
-        <v>11111</v>
-      </c>
-      <c r="G5" s="0" t="n">
-        <v>11111</v>
+      <c r="E5" s="0">
+        <f>SUMIFS('Sales and Inv Paste'!$V:$V, 'Sales and Inv Paste'!$E:$E, $B$4, 'Sales and Inv Paste'!$G:$G, $E$3, 'Sales and Inv Paste'!$J:$J, E$4, 'Sales and Inv Paste'!$K:$K, $A$5)</f>
+        <v/>
+      </c>
+      <c r="F5" s="0">
+        <f>SUMIFS('Sales and Inv Paste'!$V:$V, 'Sales and Inv Paste'!$E:$E, $B$4, 'Sales and Inv Paste'!$G:$G, $E$3, 'Sales and Inv Paste'!$J:$J, F$4, 'Sales and Inv Paste'!$K:$K, $A$5)</f>
+        <v/>
+      </c>
+      <c r="G5" s="0">
+        <f>SUMIFS('Sales and Inv Paste'!$V:$V, 'Sales and Inv Paste'!$E:$E, $B$4, 'Sales and Inv Paste'!$G:$G, $E$3, 'Sales and Inv Paste'!$J:$J, G$4, 'Sales and Inv Paste'!$K:$K, $A$5)</f>
+        <v/>
       </c>
     </row>
     <row r="6">
-      <c r="E6" s="0" t="n">
-        <v>43434</v>
+      <c r="E6" s="0" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> </t>
+        </is>
       </c>
       <c r="F6" s="0" t="n">
         <v>43434</v>
@@ -388,25 +393,31 @@
       </c>
     </row>
     <row r="7">
-      <c r="E7" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>21</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>21</v>
+      <c r="E7" s="0">
+        <f>SUMIFS('Sales and Inv Paste'!$W:$W, 'Sales and Inv Paste'!$E:$E, $B$4, 'Sales and Inv Paste'!$G:$G, $E$3, 'Sales and Inv Paste'!$J:$J, E$4, 'Sales and Inv Paste'!$K:$K, $A$5)</f>
+        <v/>
+      </c>
+      <c r="F7" s="0">
+        <f>SUMIFS('Sales and Inv Paste'!$W:$W, 'Sales and Inv Paste'!$E:$E, $B$4, 'Sales and Inv Paste'!$G:$G, $E$3, 'Sales and Inv Paste'!$J:$J, F$4, 'Sales and Inv Paste'!$K:$K, $A$5)</f>
+        <v/>
+      </c>
+      <c r="G7" s="0">
+        <f>SUMIFS('Sales and Inv Paste'!$W:$W, 'Sales and Inv Paste'!$E:$E, $B$4, 'Sales and Inv Paste'!$G:$G, $E$3, 'Sales and Inv Paste'!$J:$J, G$4, 'Sales and Inv Paste'!$K:$K, $A$5)</f>
+        <v/>
       </c>
     </row>
     <row r="8">
-      <c r="E8" s="0" t="n">
-        <v>6565</v>
-      </c>
-      <c r="F8" s="0" t="n">
-        <v>6565</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>6565</v>
+      <c r="E8" s="0">
+        <f>IFERROR((E5-E7)/E7,0)</f>
+        <v/>
+      </c>
+      <c r="F8" s="0">
+        <f>IFERROR((F5-F7)/F7,0)</f>
+        <v/>
+      </c>
+      <c r="G8" s="0">
+        <f>IFERROR((G5-G7)/G7,0)</f>
+        <v/>
       </c>
     </row>
     <row r="9"/>

</xml_diff>